<commit_message>
Add entity class for user inputs, update class name for reading and processing excel, update excel sheet
</commit_message>
<xml_diff>
--- a/ERStudio.xlsx
+++ b/ERStudio.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69225E83-3E1A-4F73-A49D-30C3B7FFEDA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +32,6 @@
     <t>String to replace</t>
   </si>
   <si>
-    <t>C:\Idera\ERStudioFiles\abc.txt</t>
-  </si>
-  <si>
     <t>C:\Idera\ERStudioFiles\xyz.txt</t>
   </si>
   <si>
@@ -50,12 +48,15 @@
   </si>
   <si>
     <t>&lt;old.major.minor&gt;</t>
+  </si>
+  <si>
+    <t>\team_server_installer\TeamServer_Bootstrapper\Config.wxi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,6 +181,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -215,6 +233,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -390,22 +425,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="52.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,38 +457,38 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
read excel row wise and update version number in each file
</commit_message>
<xml_diff>
--- a/ERStudio.xlsx
+++ b/ERStudio.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69225E83-3E1A-4F73-A49D-30C3B7FFEDA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>S.No.</t>
   </si>
@@ -32,31 +31,43 @@
     <t>String to replace</t>
   </si>
   <si>
-    <t>C:\Idera\ERStudioFiles\xyz.txt</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>&lt;old.major.minor&gt;</t>
-  </si>
-  <si>
-    <t>\team_server_installer\TeamServer_Bootstrapper\Config.wxi</t>
+    <t>MajorMinorPatch</t>
+  </si>
+  <si>
+    <t>Major.Minor</t>
+  </si>
+  <si>
+    <t>Major,Minor,Patch,0</t>
+  </si>
+  <si>
+    <t>Major,Minor,Patch,BuildNumberUpdate</t>
+  </si>
+  <si>
+    <t>Major.Minor.Patch</t>
+  </si>
+  <si>
+    <t>Major, Minor, Patch, BuildNumberUpdate</t>
+  </si>
+  <si>
+    <t>\Config.wxi</t>
+  </si>
+  <si>
+    <t>\config.wxi</t>
+  </si>
+  <si>
+    <t>\Confoiig.wxi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,8 +97,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -181,23 +195,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -233,23 +230,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,22 +405,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="61" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="59" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,38 +437,106 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
File version changes enhancement.
</commit_message>
<xml_diff>
--- a/ERStudio.xlsx
+++ b/ERStudio.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="21000" windowHeight="8615"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TS Version" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
   <si>
     <t>S.No.</t>
   </si>
@@ -89,25 +89,50 @@
     <t>team_server_installer\TeamServer_Bootstrapper\TeamServerBundle.wxs</t>
   </si>
   <si>
+    <t>team_server_installer\Prerequisites\UninstallPreviousVersion.bat</t>
+  </si>
+  <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>\TeamServerBackup_MSI\Prerequisities\UninstallPreviousVersion.bat</t>
-  </si>
-  <si>
-    <t>Major, Minor, Patch, BuildNumber</t>
-  </si>
-  <si>
-    <t>Cannot find the file</t>
-  </si>
-  <si>
     <t>\db\db2\main_create_schema.sql</t>
   </si>
   <si>
     <t>Major, Minor, Patch</t>
   </si>
   <si>
-    <t>cannot find the folder</t>
+    <t>cannot find the folder db2</t>
+  </si>
+  <si>
+    <t>Pending Items</t>
+  </si>
+  <si>
+    <t>GUID  Major Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">team_server_installer/TeamServer_MSI/Config.wxi#43
+</t>
+  </si>
+  <si>
+    <t>team_server_installer/TeamServer_Bootstrapper/Config.wxi</t>
+  </si>
+  <si>
+    <t>GUID Patch Version  - no change</t>
+  </si>
+  <si>
+    <t>GUID Major or Minor Version</t>
+  </si>
+  <si>
+    <t>need to add conditions in TeamServerBackup.wxs to consider the previous version as seamless upgrade and to take backup of required folders properly from that previous version</t>
+  </si>
+  <si>
+    <t>Need to add IDERATEAMSERVERxxxxFOLDER by looking at existing such properties</t>
+  </si>
+  <si>
+    <t>Include it in Backup* customActions</t>
+  </si>
+  <si>
+    <t>Include it in SeamLessUpgradeDetection component</t>
   </si>
 </sst>
 </file>
@@ -120,7 +145,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -140,6 +165,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -601,146 +633,150 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="19"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="19" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1088,10 +1124,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -1261,7 +1297,7 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1278,7 +1314,7 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1397,7 +1433,7 @@
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1406,8 +1442,25 @@
       <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1421,17 +1474,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2222222222222" defaultRowHeight="13.2" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="12.2222222222222" defaultRowHeight="13.2" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="11.5740740740741"/>
-    <col min="2" max="2" width="49.75"/>
-    <col min="3" max="3" width="13.037037037037"/>
+    <col min="2" max="2" width="53.3333333333333" customWidth="1"/>
+    <col min="3" max="3" width="19.3333333333333" customWidth="1"/>
     <col min="4" max="4" width="13.462962962963"/>
     <col min="5" max="5" width="17.8518518518519"/>
     <col min="6" max="6" width="30.75"/>
@@ -1455,7 +1508,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" ht="14.4" spans="1:6">
@@ -1463,39 +1516,78 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" ht="14.4" spans="1:6">
-      <c r="A3" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" ht="26.4" spans="2:2">
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>30</v>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" ht="13.8" spans="2:2">
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" ht="13.8" spans="2:2">
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update patch upgrade column for AbstractDatabaseCreator.java
</commit_message>
<xml_diff>
--- a/ERStudio.xlsx
+++ b/ERStudio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ERStudioReleaseHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9A115E-0540-42D5-A428-B28A5E93693C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A224B6-E090-494E-9AC9-86F433A68280}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
   <si>
     <t>S.No.</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Major.Minor.Patch.BuildNumber</t>
@@ -114,19 +111,22 @@
     <t>Major_Minor_Patch</t>
   </si>
   <si>
+    <t>Major.Minor.Patch</t>
+  </si>
+  <si>
+    <t>MajorMinorPatch</t>
+  </si>
+  <si>
     <t>team_server_installer\TeamServer_MSI\Config.wxi</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>team_server_installer\TeamServerBackup_MSI\Resources\UninstallPreviousVersion.bat</t>
   </si>
   <si>
     <t>build.xml</t>
-  </si>
-  <si>
-    <t>Major.Minor.Patch</t>
-  </si>
-  <si>
-    <t>MajorMinorPatch</t>
   </si>
   <si>
     <t>db\sqlserver\main_data.sql</t>
@@ -532,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ19"/>
+  <dimension ref="A1:AMJ20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E19"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,16 +570,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -587,16 +587,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -604,7 +604,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -613,7 +613,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -621,16 +621,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -638,98 +638,95 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>36</v>
@@ -737,41 +734,41 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>38</v>
@@ -780,95 +777,112 @@
         <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>7</v>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -882,13 +896,13 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.26953125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.08984375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="98.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="16.36328125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12.54296875" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="33.81640625" customWidth="1" collapsed="1"/>
@@ -897,7 +911,7 @@
     <row r="1" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -906,7 +920,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
@@ -914,13 +928,13 @@
         <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>43</v>
@@ -937,7 +951,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>43</v>
@@ -945,24 +959,24 @@
     </row>
     <row r="4" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1005,12 +1019,12 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1018,17 +1032,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1036,7 +1050,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1044,27 +1058,27 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1072,17 +1086,17 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change custom data for patchRepo in ERStudio.xlsx
</commit_message>
<xml_diff>
--- a/ERStudio.xlsx
+++ b/ERStudio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ERStudioReleaseHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42514BEE-14CD-4E33-BD7F-3555239282F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725E6E0A-1BAA-4E5F-B7FE-EF546D966886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="48">
   <si>
     <t>S.No.</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Version doesn't looks to be getting updated in following files.</t>
+  </si>
+  <si>
+    <t>sqlserver</t>
+  </si>
+  <si>
+    <t>oracle</t>
   </si>
 </sst>
 </file>
@@ -496,7 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -843,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -936,7 +942,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -953,7 +959,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Change custom data for patchRepo in ERStudio.xlsx"
This reverts commit e133813197de0d6d7267097d814f965d46211341.
</commit_message>
<xml_diff>
--- a/ERStudio.xlsx
+++ b/ERStudio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ERStudioReleaseHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725E6E0A-1BAA-4E5F-B7FE-EF546D966886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42514BEE-14CD-4E33-BD7F-3555239282F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="46">
   <si>
     <t>S.No.</t>
   </si>
@@ -161,12 +161,6 @@
   </si>
   <si>
     <t>Version doesn't looks to be getting updated in following files.</t>
-  </si>
-  <si>
-    <t>sqlserver</t>
-  </si>
-  <si>
-    <t>oracle</t>
   </si>
 </sst>
 </file>
@@ -502,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -849,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -942,7 +936,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -959,7 +953,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>